<commit_message>
se modifican seccion de direccion de la compañia
</commit_message>
<xml_diff>
--- a/static/files/city.xlsx
+++ b/static/files/city.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">state</t>
   </si>
@@ -28,10 +28,13 @@
     <t xml:space="preserve">city</t>
   </si>
   <si>
-    <t xml:space="preserve">ALVARO OBREGON</t>
+    <t xml:space="preserve">cp</t>
   </si>
   <si>
-    <t xml:space="preserve">COMITAN DE RODRIGO</t>
+    <t xml:space="preserve">miguel hidalgo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">xochimilco </t>
   </si>
 </sst>
 </file>
@@ -128,10 +131,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -150,21 +153,30 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>11000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>16000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>